<commit_message>
Fix for application.py flask
</commit_message>
<xml_diff>
--- a/temporary_file.xlsx
+++ b/temporary_file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,48 +434,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
-    <col width="19" customWidth="1" min="5" max="5"/>
-    <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="19" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Alumno</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Curso A Predicted</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Curso B Predicted</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Curso C Predicted</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Curso D Predicted</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Curso E Predicted</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Curso F Predicted</t>
         </is>
       </c>
     </row>
@@ -485,24 +449,6 @@
           <t>Mark</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>12.51</v>
-      </c>
-      <c r="C2" t="n">
-        <v>12.51</v>
-      </c>
-      <c r="D2" t="n">
-        <v>12.51</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12.51</v>
-      </c>
-      <c r="F2" t="n">
-        <v>12.51</v>
-      </c>
-      <c r="G2" t="n">
-        <v>12.51</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -510,24 +456,6 @@
           <t>Jose</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="C3" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="D3" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="E3" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="F3" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="G3" t="n">
-        <v>13.11</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add application flask name
</commit_message>
<xml_diff>
--- a/temporary_file.xlsx
+++ b/temporary_file.xlsx
@@ -468,13 +468,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14.37</v>
+        <v>14.09</v>
       </c>
       <c r="C2" t="n">
-        <v>12.98</v>
+        <v>13.72</v>
       </c>
       <c r="D2" t="n">
-        <v>10.74</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14.32</v>
+        <v>13.87</v>
       </c>
       <c r="C3" t="n">
-        <v>12.82</v>
+        <v>13.57</v>
       </c>
       <c r="D3" t="n">
-        <v>10.65</v>
+        <v>10.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>